<commit_message>
Emparrillado en el informe
</commit_message>
<xml_diff>
--- a/3- Emparrillado/Emparrillado.xlsx
+++ b/3- Emparrillado/Emparrillado.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="75">
   <si>
     <t xml:space="preserve">Fastball </t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Atrás</t>
-  </si>
-  <si>
-    <t>Adelante</t>
   </si>
   <si>
     <t>Alineados</t>
@@ -293,7 +290,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,8 +321,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -676,11 +679,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -695,36 +711,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -753,24 +742,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1067,518 +1089,524 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="4.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:11" s="4" customFormat="1">
-      <c r="B2" s="6"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="8"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="2:11" s="2" customFormat="1" ht="12.75">
-      <c r="B3" s="9"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="45" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="45" t="s">
+      <c r="E3" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="45" t="s">
+      <c r="G3" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="10"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="18">
-        <v>2</v>
-      </c>
-      <c r="E4" s="18">
-        <v>2</v>
-      </c>
-      <c r="F4" s="18">
-        <v>2</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2</v>
+      </c>
+      <c r="G4" s="9">
         <v>1</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="9">
         <v>3</v>
       </c>
-      <c r="I4" s="18">
-        <v>2</v>
-      </c>
-      <c r="J4" s="46" t="s">
+      <c r="I4" s="9">
+        <v>2</v>
+      </c>
+      <c r="J4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="49" t="s">
-        <v>23</v>
+      <c r="K4" s="51" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="46" t="s">
+      <c r="B5" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="18">
-        <v>2</v>
-      </c>
-      <c r="E5" s="18">
-        <v>2</v>
-      </c>
-      <c r="F5" s="18">
-        <v>2</v>
-      </c>
-      <c r="G5" s="47">
-        <v>2</v>
-      </c>
-      <c r="H5" s="47">
-        <v>2</v>
-      </c>
-      <c r="I5" s="47">
+      <c r="D5" s="9">
+        <v>2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>2</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2</v>
+      </c>
+      <c r="G5" s="35">
+        <v>2</v>
+      </c>
+      <c r="H5" s="35">
+        <v>2</v>
+      </c>
+      <c r="I5" s="35">
         <v>1</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="49" t="s">
-        <v>20</v>
+      <c r="K5" s="51" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="18">
-        <v>2</v>
-      </c>
-      <c r="E6" s="18">
-        <v>2</v>
-      </c>
-      <c r="F6" s="18">
-        <v>2</v>
-      </c>
-      <c r="G6" s="47">
-        <v>2</v>
-      </c>
-      <c r="H6" s="47">
+      <c r="D6" s="9">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9">
+        <v>2</v>
+      </c>
+      <c r="G6" s="35">
+        <v>2</v>
+      </c>
+      <c r="H6" s="35">
         <v>1</v>
       </c>
-      <c r="I6" s="47">
+      <c r="I6" s="35">
         <v>3</v>
       </c>
-      <c r="J6" s="46" t="s">
+      <c r="J6" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="49" t="s">
-        <v>19</v>
+      <c r="K6" s="51" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="23">
+        <v>2</v>
+      </c>
+      <c r="E7" s="23">
+        <v>1</v>
+      </c>
+      <c r="F7" s="23">
+        <v>3</v>
+      </c>
+      <c r="G7" s="23">
+        <v>2</v>
+      </c>
+      <c r="H7" s="23">
+        <v>2</v>
+      </c>
+      <c r="I7" s="23">
+        <v>3</v>
+      </c>
+      <c r="J7" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="32">
-        <v>2</v>
-      </c>
-      <c r="E7" s="32">
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="23">
         <v>1</v>
       </c>
-      <c r="F7" s="32">
+      <c r="E8" s="23">
+        <v>1</v>
+      </c>
+      <c r="F8" s="23">
+        <v>4</v>
+      </c>
+      <c r="G8" s="23">
         <v>3</v>
       </c>
-      <c r="G7" s="32">
-        <v>2</v>
-      </c>
-      <c r="H7" s="32">
-        <v>2</v>
-      </c>
-      <c r="I7" s="32">
+      <c r="H8" s="23">
+        <v>2</v>
+      </c>
+      <c r="I8" s="23">
+        <v>4</v>
+      </c>
+      <c r="J8" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B9" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="36">
         <v>3</v>
       </c>
-      <c r="J7" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="49" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="32">
+      <c r="E9" s="36">
         <v>1</v>
       </c>
-      <c r="E8" s="32">
-        <v>1</v>
-      </c>
-      <c r="F8" s="32">
-        <v>4</v>
-      </c>
-      <c r="G8" s="32">
-        <v>3</v>
-      </c>
-      <c r="H8" s="32">
-        <v>2</v>
-      </c>
-      <c r="I8" s="32">
-        <v>4</v>
-      </c>
-      <c r="J8" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B9" s="50" t="s">
+      <c r="F9" s="36">
+        <v>2</v>
+      </c>
+      <c r="G9" s="36">
+        <v>2</v>
+      </c>
+      <c r="H9" s="36">
+        <v>2</v>
+      </c>
+      <c r="I9" s="36">
+        <v>2</v>
+      </c>
+      <c r="J9" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="52" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="52">
-        <v>3</v>
-      </c>
-      <c r="E9" s="52">
-        <v>1</v>
-      </c>
-      <c r="F9" s="52">
-        <v>2</v>
-      </c>
-      <c r="G9" s="52">
-        <v>2</v>
-      </c>
-      <c r="H9" s="52">
-        <v>2</v>
-      </c>
-      <c r="I9" s="52">
-        <v>2</v>
-      </c>
-      <c r="J9" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="53" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B11" s="14" t="s">
-        <v>33</v>
+    <row r="11" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B11" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="16">
+      <c r="E11" s="8">
         <v>1</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="8" t="s">
         <v>18</v>
       </c>
       <c r="J11" s="2"/>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="2:11" s="16" customFormat="1" ht="12.75">
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B12" s="5"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="16">
-        <v>2</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>22</v>
+      <c r="E12" s="8">
+        <v>2</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="J12" s="2"/>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="2:11" s="16" customFormat="1" ht="12.75">
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B13" s="5"/>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="16">
+      <c r="E13" s="8">
         <v>3</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>23</v>
+      <c r="F13" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="K13" s="15"/>
-    </row>
-    <row r="14" spans="2:11" s="16" customFormat="1" ht="12.75">
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B14" s="5"/>
       <c r="C14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="15"/>
-    </row>
-    <row r="15" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B15" s="15" t="s">
-        <v>24</v>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B15" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="E15" s="16">
+      <c r="E15" s="8">
         <v>1</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>21</v>
+      <c r="F15" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="J15" s="2"/>
-      <c r="K15" s="15"/>
-    </row>
-    <row r="16" spans="2:11" s="16" customFormat="1" ht="12.75">
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B16" s="5"/>
       <c r="C16" s="2"/>
-      <c r="E16" s="16">
-        <v>2</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>20</v>
+      <c r="E16" s="8">
+        <v>2</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="J16" s="2"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="2:11" s="16" customFormat="1" ht="12.75">
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="2:11" s="8" customFormat="1" ht="12.75">
       <c r="B17" s="5"/>
       <c r="C17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B18" s="15" t="s">
-        <v>25</v>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B18" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="E18" s="16">
+      <c r="E18" s="8">
         <v>1</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="8" t="s">
         <v>18</v>
       </c>
       <c r="J18" s="2"/>
-      <c r="K18" s="15"/>
-    </row>
-    <row r="19" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B19" s="15"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B19" s="7"/>
       <c r="C19" s="2"/>
-      <c r="E19" s="16">
-        <v>2</v>
-      </c>
-      <c r="F19" s="16" t="s">
+      <c r="E19" s="8">
+        <v>2</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B20" s="7"/>
+      <c r="C20" s="2"/>
+      <c r="E20" s="8">
+        <v>3</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="15"/>
-    </row>
-    <row r="20" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B20" s="15"/>
-      <c r="C20" s="2"/>
-      <c r="E20" s="16">
-        <v>3</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="J20" s="2"/>
-      <c r="K20" s="15"/>
-    </row>
-    <row r="21" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B21" s="15"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B21" s="7"/>
       <c r="C21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="15"/>
-    </row>
-    <row r="22" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B22" s="15" t="s">
-        <v>34</v>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B22" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="E22" s="16">
+      <c r="E22" s="8">
         <v>1</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B23" s="7"/>
+      <c r="C23" s="28"/>
+      <c r="E23" s="8">
+        <v>2</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="28"/>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B24" s="7"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="8">
+        <v>3</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="23" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B23" s="15"/>
-      <c r="C23" s="37"/>
-      <c r="E23" s="16">
-        <v>2</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="37"/>
-      <c r="K23" s="15"/>
-    </row>
-    <row r="24" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B24" s="15"/>
-      <c r="C24" s="2"/>
-      <c r="E24" s="16">
-        <v>3</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>74</v>
-      </c>
       <c r="J24" s="2"/>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B25" s="15"/>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B25" s="7"/>
       <c r="C25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B26" s="15" t="s">
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="E26" s="8">
+        <v>1</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B27" s="7"/>
+      <c r="C27" s="2"/>
+      <c r="E27" s="8">
+        <v>2</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="E26" s="16">
-        <v>1</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J26" s="2"/>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B27" s="15"/>
-      <c r="C27" s="2"/>
-      <c r="E27" s="16">
-        <v>2</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>28</v>
-      </c>
       <c r="J27" s="2"/>
-      <c r="K27" s="15"/>
-    </row>
-    <row r="28" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B28" s="15"/>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B28" s="7"/>
       <c r="C28" s="2"/>
-      <c r="E28" s="16">
+      <c r="E28" s="8">
         <v>3</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>31</v>
+      <c r="F28" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="J28" s="2"/>
-      <c r="K28" s="15"/>
-    </row>
-    <row r="29" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B29" s="15"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B29" s="7"/>
       <c r="C29" s="2"/>
-      <c r="E29" s="16">
-        <v>4</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>30</v>
+      <c r="E29" s="8">
+        <v>4</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="J29" s="2"/>
-      <c r="K29" s="15"/>
-    </row>
-    <row r="30" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B30" s="15"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B30" s="7"/>
       <c r="C30" s="2"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="15"/>
-    </row>
-    <row r="31" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B31" s="15" t="s">
-        <v>35</v>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B31" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="E31" s="16">
+      <c r="E31" s="8">
         <v>1</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="2:11" s="8" customFormat="1" ht="12.75">
+      <c r="B32" s="7"/>
+      <c r="C32" s="2"/>
+      <c r="E32" s="8">
+        <v>2</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="5:6">
+      <c r="E33" s="8">
+        <v>3</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="J31" s="2"/>
-      <c r="K31" s="15"/>
-    </row>
-    <row r="32" spans="2:11" s="16" customFormat="1" ht="12.75">
-      <c r="B32" s="15"/>
-      <c r="C32" s="2"/>
-      <c r="E32" s="16">
-        <v>2</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="15"/>
-    </row>
-    <row r="33" spans="5:6">
-      <c r="E33" s="16">
-        <v>3</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1591,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1602,8 +1630,7 @@
     <col min="3" max="3" width="1.85546875" customWidth="1"/>
     <col min="4" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="7" max="10" width="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.7109375" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1612,17 +1639,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="44"/>
+      <c r="A1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="55"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <f>ABS(Emparrillado!D4-Emparrillado!E4)+ABS(Emparrillado!D5-Emparrillado!E5)+ABS(Emparrillado!D6-Emparrillado!E6)+ABS(Emparrillado!D7-Emparrillado!E7)+ABS(Emparrillado!D8-Emparrillado!E8)+ABS(Emparrillado!D9-Emparrillado!E9)</f>
@@ -1631,250 +1658,250 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <f>ABS(Emparrillado!D4-Emparrillado!F4)+ABS(Emparrillado!D5-Emparrillado!F5)+ABS(Emparrillado!D6-Emparrillado!F6)+ABS(Emparrillado!D7-Emparrillado!F7)+ABS(Emparrillado!D8-Emparrillado!F8)+ ABS(Emparrillado!D9-Emparrillado!F9)</f>
         <v>5</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="38" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="G4" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="H4" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="I4" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="39" t="s">
+      <c r="J4" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="31" t="s">
+      <c r="L4" s="9"/>
+      <c r="M4" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="N4" s="31" t="s">
+      <c r="O4" s="22" t="s">
         <v>61</v>
-      </c>
-      <c r="O4" s="31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <f>ABS(Emparrillado!D4-Emparrillado!G4)+ABS(Emparrillado!D5-Emparrillado!G5)+ABS(Emparrillado!D6-Emparrillado!G6)+ABS(Emparrillado!D7-Emparrillado!G7)+ABS(Emparrillado!D8-Emparrillado!G8)+ABS(Emparrillado!D9-Emparrillado!G9)</f>
         <v>4</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="27">
+      <c r="D5" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="18">
         <f>B3</f>
         <v>3</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="19">
         <f>B4</f>
         <v>5</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="16">
         <f>B5</f>
         <v>4</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="16">
         <f>B6</f>
         <v>4</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="25">
         <f>B7</f>
         <v>7</v>
       </c>
-      <c r="L5" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="18">
-        <v>4</v>
-      </c>
-      <c r="N5" s="18">
+      <c r="L5" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="9">
+        <v>4</v>
+      </c>
+      <c r="N5" s="9">
         <v>7</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="9">
         <f>MIN(M5:N5)</f>
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <f>ABS(Emparrillado!D4-Emparrillado!H4)+ABS(Emparrillado!D5-Emparrillado!H5)+ABS(Emparrillado!D6-Emparrillado!H6)+ABS(Emparrillado!D7-Emparrillado!H7)+ABS(Emparrillado!D8-Emparrillado!H8)+ABS(Emparrillado!D9-Emparrillado!H9)</f>
         <v>4</v>
       </c>
-      <c r="D6" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="29">
+      <c r="D6" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="20">
         <f>B8</f>
         <v>6</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="9">
         <f>B9</f>
         <v>5</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="9">
         <f>B10</f>
         <v>5</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="21">
         <f>B11</f>
         <v>8</v>
       </c>
-      <c r="L6" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="M6" s="18">
+      <c r="L6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="9">
         <v>6</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="9">
         <v>8</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="9">
         <f t="shared" ref="O6:O8" si="0">MIN(M6:N6)</f>
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <f>ABS(Emparrillado!D4-Emparrillado!I4)+ABS(Emparrillado!D5-Emparrillado!I5)+ABS(Emparrillado!D6-Emparrillado!I6)+ABS(Emparrillado!D7-Emparrillado!I7)+ABS(Emparrillado!D8-Emparrillado!I8)+ABS(Emparrillado!D9-Emparrillado!I9)</f>
         <v>7</v>
       </c>
-      <c r="D7" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="33">
+      <c r="D7" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="24">
         <f>B12</f>
         <v>3</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="24">
         <f>B13</f>
         <v>5</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="26">
         <f>B14</f>
         <v>2</v>
       </c>
-      <c r="L7" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="M7" s="18">
+      <c r="L7" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="9">
         <v>3</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="9">
         <v>5</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <f>ABS(Emparrillado!E4-Emparrillado!F4)+ABS(Emparrillado!E5-Emparrillado!F5)+ABS(Emparrillado!E6-Emparrillado!F6)+ABS(Emparrillado!E7-Emparrillado!F7)+ABS(Emparrillado!E8-Emparrillado!F8)+ ABS(Emparrillado!E9-Emparrillado!F9)</f>
         <v>6</v>
       </c>
-      <c r="D8" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="18">
+      <c r="D8" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="9">
         <f>B15</f>
         <v>4</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="21">
         <f>B16</f>
         <v>5</v>
       </c>
-      <c r="L8" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="M8" s="18">
+      <c r="L8" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" s="9">
         <v>5</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="9">
         <v>7</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <f>ABS(Emparrillado!E4-Emparrillado!G4)+ABS(Emparrillado!E5-Emparrillado!G5)+ABS(Emparrillado!E6-Emparrillado!G6)+ABS(Emparrillado!E7-Emparrillado!G7)+ABS(Emparrillado!E8-Emparrillado!G8)+ABS(Emparrillado!E9-Emparrillado!G9)</f>
         <v>5</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="30">
+      <c r="D9" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="21">
         <f>B17</f>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <f>ABS(Emparrillado!E4-Emparrillado!H4)+ABS(Emparrillado!E5-Emparrillado!H5)+ABS(Emparrillado!E6-Emparrillado!H6)+ABS(Emparrillado!E7-Emparrillado!H7)+ABS(Emparrillado!E8-Emparrillado!H8)+ABS(Emparrillado!E9-Emparrillado!H9)</f>
         <v>5</v>
       </c>
-      <c r="D10" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="21"/>
+      <c r="D10" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11">
         <f>ABS(Emparrillado!E4-Emparrillado!I4)+ABS(Emparrillado!E5-Emparrillado!I5)+ABS(Emparrillado!E6-Emparrillado!I6)+ABS(Emparrillado!E7-Emparrillado!I7)+ABS(Emparrillado!E8-Emparrillado!I8)+ABS(Emparrillado!E9-Emparrillado!I9)</f>
@@ -1883,383 +1910,383 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <f>ABS(Emparrillado!F4-Emparrillado!G4)+ABS(Emparrillado!F5-Emparrillado!G5)+ABS(Emparrillado!F6-Emparrillado!G6)+ABS(Emparrillado!F7-Emparrillado!G7)+ABS(Emparrillado!F8-Emparrillado!G8)+ABS(Emparrillado!F9-Emparrillado!G9)</f>
         <v>3</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="31" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="L12" s="18"/>
-      <c r="M12" s="31" t="s">
+      <c r="L12" s="9"/>
+      <c r="M12" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="N12" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="O12" s="31" t="s">
-        <v>62</v>
+      <c r="O12" s="22" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <f>ABS(Emparrillado!F4-Emparrillado!H4)+ABS(Emparrillado!F5-Emparrillado!H5)+ABS(Emparrillado!F6-Emparrillado!H6)+ABS(Emparrillado!F7-Emparrillado!H7)+ABS(Emparrillado!F8-Emparrillado!H8)+ABS(Emparrillado!F9-Emparrillado!H9)</f>
         <v>5</v>
       </c>
-      <c r="D13" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="29">
+      <c r="D13" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="20">
         <f>O5</f>
         <v>4</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="20">
         <f>O6</f>
         <v>6</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="23">
         <f>O7</f>
         <v>3</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="23">
         <f>O8</f>
         <v>5</v>
       </c>
-      <c r="L13" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="M13" s="18">
-        <v>4</v>
-      </c>
-      <c r="N13" s="18">
+      <c r="L13" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" s="9">
+        <v>4</v>
+      </c>
+      <c r="N13" s="9">
         <v>6</v>
       </c>
-      <c r="O13" s="18">
+      <c r="O13" s="9">
         <f>MIN(M13:N13)</f>
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <f>ABS(Emparrillado!F4-Emparrillado!I4)+ABS(Emparrillado!F5-Emparrillado!I5)+ABS(Emparrillado!F6-Emparrillado!I6)+ABS(Emparrillado!F7-Emparrillado!I7)+ABS(Emparrillado!F8-Emparrillado!I8)+ABS(Emparrillado!F9-Emparrillado!I9)</f>
         <v>2</v>
       </c>
-      <c r="D14" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="36">
+      <c r="D14" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="27">
         <v>3</v>
       </c>
-      <c r="H14" s="29">
-        <v>4</v>
-      </c>
-      <c r="I14" s="29">
-        <v>4</v>
-      </c>
-      <c r="L14" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="M14" s="18">
-        <v>4</v>
-      </c>
-      <c r="N14" s="18">
+      <c r="H14" s="20">
+        <v>4</v>
+      </c>
+      <c r="I14" s="20">
+        <v>4</v>
+      </c>
+      <c r="L14" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="9">
+        <v>4</v>
+      </c>
+      <c r="N14" s="9">
         <v>5</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O14" s="9">
         <f t="shared" ref="O14:O15" si="1">MIN(M14:N14)</f>
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <f>ABS(Emparrillado!G4-Emparrillado!H4)+ABS(Emparrillado!G5-Emparrillado!H5)+ABS(Emparrillado!G6-Emparrillado!H6)+ABS(Emparrillado!G7-Emparrillado!H7)+ABS(Emparrillado!G8-Emparrillado!H8)+ABS(Emparrillado!G9-Emparrillado!H9)</f>
         <v>4</v>
       </c>
-      <c r="D15" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="29">
+      <c r="D15" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="20">
         <v>5</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="20">
         <v>5</v>
       </c>
-      <c r="L15" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" s="18">
-        <v>4</v>
-      </c>
-      <c r="N15" s="18">
+      <c r="L15" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="M15" s="9">
+        <v>4</v>
+      </c>
+      <c r="N15" s="9">
         <v>5</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O15" s="9">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <f>ABS(Emparrillado!G4-Emparrillado!I4)+ABS(Emparrillado!G5-Emparrillado!I5)+ABS(Emparrillado!G6-Emparrillado!I6)+ABS(Emparrillado!G7-Emparrillado!I7)+ABS(Emparrillado!G8-Emparrillado!I8)+ABS(Emparrillado!G9-Emparrillado!I9)</f>
         <v>5</v>
       </c>
-      <c r="D16" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="32">
+      <c r="D16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="23">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <f>ABS(Emparrillado!H4-Emparrillado!I4)+ABS(Emparrillado!H5-Emparrillado!I5)+ABS(Emparrillado!H6-Emparrillado!I6)+ABS(Emparrillado!H7-Emparrillado!I7)+ABS(Emparrillado!H8-Emparrillado!I8)+ABS(Emparrillado!H9-Emparrillado!I9)</f>
         <v>7</v>
       </c>
-      <c r="D17" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="19"/>
+      <c r="D17" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="D19" s="18"/>
-      <c r="E19" s="31" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L19" s="9"/>
+      <c r="M19" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="O19" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="D20" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="20">
+        <f>O13</f>
+        <v>4</v>
+      </c>
+      <c r="G20" s="20">
+        <f>O14</f>
+        <v>4</v>
+      </c>
+      <c r="H20" s="23">
+        <f>O15</f>
+        <v>4</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="M20" s="9">
+        <v>4</v>
+      </c>
+      <c r="N20" s="9">
+        <v>4</v>
+      </c>
+      <c r="O20" s="9">
+        <f t="shared" ref="O20:O21" si="2">MIN(M20:N20)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="D21" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="27">
+        <v>3</v>
+      </c>
+      <c r="H21" s="20">
+        <v>5</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21" s="9">
+        <v>5</v>
+      </c>
+      <c r="N21" s="9">
+        <v>4</v>
+      </c>
+      <c r="O21" s="9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="D22" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="D23" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="D25" s="9"/>
+      <c r="E25" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L25" s="9"/>
+      <c r="M25" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="O25" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="D26" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="20">
+        <f>O20</f>
+        <v>4</v>
+      </c>
+      <c r="G26" s="20">
+        <f>O21</f>
+        <v>4</v>
+      </c>
+      <c r="L26" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="M26" s="9">
+        <v>4</v>
+      </c>
+      <c r="N26" s="9">
+        <v>4</v>
+      </c>
+      <c r="O26" s="9">
+        <f t="shared" ref="O26" si="3">MIN(M26:N26)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="D27" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="D28" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="D30" s="9"/>
+      <c r="E30" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="N19" s="31" t="s">
+      <c r="F30" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="O19" s="31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="D20" s="31" t="s">
+    </row>
+    <row r="31" spans="1:15">
+      <c r="D31" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="29">
-        <f>O13</f>
-        <v>4</v>
-      </c>
-      <c r="G20" s="29">
-        <f>O14</f>
-        <v>4</v>
-      </c>
-      <c r="H20" s="32">
-        <f>O15</f>
-        <v>4</v>
-      </c>
-      <c r="L20" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="M20" s="18">
-        <v>4</v>
-      </c>
-      <c r="N20" s="18">
-        <v>4</v>
-      </c>
-      <c r="O20" s="18">
-        <f t="shared" ref="O20:O21" si="2">MIN(M20:N20)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="D21" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="36">
-        <v>3</v>
-      </c>
-      <c r="H21" s="29">
-        <v>5</v>
-      </c>
-      <c r="L21" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="M21" s="18">
-        <v>5</v>
-      </c>
-      <c r="N21" s="18">
-        <v>4</v>
-      </c>
-      <c r="O21" s="18">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="D22" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="D23" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="D25" s="18"/>
-      <c r="E25" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="L25" s="18"/>
-      <c r="M25" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="N25" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="O25" s="31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="D26" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="29">
-        <f>O20</f>
-        <v>4</v>
-      </c>
-      <c r="G26" s="29">
-        <f>O21</f>
-        <v>4</v>
-      </c>
-      <c r="L26" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="M26" s="18">
-        <v>4</v>
-      </c>
-      <c r="N26" s="18">
-        <v>4</v>
-      </c>
-      <c r="O26" s="18">
-        <f t="shared" ref="O26" si="3">MIN(M26:N26)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="D27" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="18"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="D28" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="D30" s="18"/>
-      <c r="E30" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="D31" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="36">
+      <c r="E31" s="10"/>
+      <c r="F31" s="27">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="D32" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="19"/>
+      <c r="D32" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="15"/>
+      <c r="A53" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>